<commit_message>
change the table formating
</commit_message>
<xml_diff>
--- a/andela_class2a_names.xlsx
+++ b/andela_class2a_names.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OBA\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OBA\team-justise\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -198,7 +198,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,8 +218,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,8 +239,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -256,17 +268,111 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -274,11 +380,212 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right/>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -289,6 +596,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D26" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5" headerRowCellStyle="Good">
+  <autoFilter ref="A1:D26"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="S/N" dataDxfId="4"/>
+    <tableColumn id="2" name="Name" dataDxfId="3"/>
+    <tableColumn id="3" name="Email" dataDxfId="2"/>
+    <tableColumn id="4" name="Avatar(Yes)" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -557,27 +877,33 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D26"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -586,10 +912,10 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -598,12 +924,12 @@
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -612,12 +938,12 @@
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -626,12 +952,12 @@
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -640,12 +966,12 @@
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -654,12 +980,12 @@
       <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -668,12 +994,12 @@
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -682,12 +1008,12 @@
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -696,26 +1022,26 @@
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -724,12 +1050,12 @@
       <c r="C12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -738,12 +1064,12 @@
       <c r="C13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -752,12 +1078,12 @@
       <c r="C14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -766,10 +1092,10 @@
       <c r="C15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -778,12 +1104,12 @@
       <c r="C16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -792,12 +1118,12 @@
       <c r="C17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -806,12 +1132,12 @@
       <c r="C18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -820,12 +1146,12 @@
       <c r="C19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+      <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -834,12 +1160,12 @@
       <c r="C20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -848,26 +1174,26 @@
       <c r="C21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -876,12 +1202,12 @@
       <c r="C23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+      <c r="A24" s="4">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -890,10 +1216,10 @@
       <c r="C24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -902,26 +1228,29 @@
       <c r="C25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
+      <c r="D25" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="8" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>